<commit_message>
Make the participant import more resilient to hand-crafted spreadsheets
</commit_message>
<xml_diff>
--- a/tests/resources/event_participation_export-noScoutNameColumn.xlsx
+++ b/tests/resources/event_participation_export-noScoutNameColumn.xlsx
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$W$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$C$1:$W$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +29,7 @@
     <t xml:space="preserve">Vorname</t>
   </si>
   <si>
-    <t xml:space="preserve">Pfadiname</t>
+    <t xml:space="preserve">Nachname</t>
   </si>
   <si>
     <t xml:space="preserve">Firmenname</t>
@@ -190,6 +191,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -208,13 +210,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
@@ -266,7 +268,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,23 +278,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -302,29 +304,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.89"/>
@@ -337,8 +339,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="25.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="22.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="24" style="0" width="9.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>